<commit_message>
Teste de sistema concluido
</commit_message>
<xml_diff>
--- a/Java/TestedeSistema.xlsx
+++ b/Java/TestedeSistema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csf14\Desktop\verival2Trab1\VeriVal2\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A34546B-99B3-4F18-8C99-4E956BC62E30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60489688-DCCE-47B8-8078-09787100A9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2DA30366-0FAA-42A7-BFD2-EF0DC84B3127}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>Descrição</t>
   </si>
@@ -75,9 +75,6 @@
     <t xml:space="preserve">O programa mostra a lista de alocações existentes apartir de um periodo de tempo fornecido pelo usuario, com as informações do medico responsavel, informações da sala usada e as datas de inicio e fim. </t>
   </si>
   <si>
-    <t xml:space="preserve">Após o usuario informar em qual periodo de tempo deseja visualizar a lista de alocações, o programa mostra todas alocações existentes nesse periodo, tanto passadas quanto futuros, com todas as informações necessarias. </t>
-  </si>
-  <si>
     <t>O usuario deve requisitar a lista da relação dos medicos e seus gastos, inserindo o numero 4 no menu.</t>
   </si>
   <si>
@@ -112,6 +109,93 @@
   </si>
   <si>
     <t>A alocação seleciona foi excluida com sucesso.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/11/10/30 e final como 2023/10/11/13/30.</t>
+  </si>
+  <si>
+    <t>O programa deve fazer a reserva com sucesso</t>
+  </si>
+  <si>
+    <t>Após todos os passos efetuados pelo usuario, o programa confirma a reserva do mesmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Após o usuario informar em qual periodo de tempo deseja visualizar a lista de alocações, o programa mostra todas alocações existentes no programa, tanto passadas quanto futuros, com todas as informações necessarias. </t>
+  </si>
+  <si>
+    <t>Sucesso, mas precisa revisão</t>
+  </si>
+  <si>
+    <t>Após revisão(Caso tivesse bug)</t>
+  </si>
+  <si>
+    <t>O programa agora filtra corretamente a lista de alocações de determinado periodo de tempo desejado</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/10/10/10 e final como 2023/10/10/11/10.</t>
+  </si>
+  <si>
+    <t>O programa deve impedir que o usuario faça a reserva</t>
+  </si>
+  <si>
+    <t>Após confirmar as datas da alocação, o programa recusa a reserva e lança uma mensagem do ocorrido</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/10/10/10 e final como 2023/10/10/12/10.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 1 na lista, e por fim, escolher a data inicial como 2023/10/10/10/10 e final como 2023/10/10/12/20.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 0 na lista, depois a sala de posição 2 na lista, e por fim, escolher a data inicial como 2023/10/10/10/10 e final como 2023/10/10/11/12</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 0 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/10/10/10 e final como 2023/10/10/12/40</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 0 na lista, depois a sala de posição 1 na lista, e por fim, escolher a data inicial como 2023/10/10/10/10 e final como 2023/10/10/12/12</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/12/10/10 e final como 2023/10/12/12/10.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 1 na lista, e por fim, escolher a data inicial como 2023/10/17/10/10 e final como 2023/10/17/12/20.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 1 na lista, e por fim, escolher a data inicial como 2023/10/18/10/10 e final como 2023/10/18/11/20.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 2 na lista, e por fim, escolher a data inicial como 2023/10/18/10/10 e final como 2023/10/18/12/20.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 1 na lista, e por fim, escolher a data inicial como 2023/10/20/10/10 e final como 2023/10/20/11/20.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 2 na lista, e por fim, escolher a data inicial como 2023/10/20/10/10 e final como 2023/10/20/12/20</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 0 na lista, depois a sala de posição 2 na lista, e por fim, escolher a data inicial como 2023/10/13/10/10 e final como 2023/10/13/12/30</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/14/10/10 e final como 2023/10/14/13/12.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/15/10/10 e final como 2023/10/15/11/10.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/19/5/10 e final como 2023/10/19/12/20.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 2 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2023/10/19/10/10 e final como 2023/10/19/23/20</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 0 na lista, e por fim, escolher a data inicial como 2020/05/12/10/30 e final como 2020/05/12/13/40</t>
+  </si>
+  <si>
+    <t>O usuario deve tentar excluir a alocação que corresponda a data atual e que esteja num periodo de tempo que inclua o atual horario, inserindo o numero 7 no menu.</t>
+  </si>
+  <si>
+    <t>O programa deve informar ao usuario que não é possivel excluir essa alocação, visto que está ocorrendo e impedi-la.</t>
   </si>
 </sst>
 </file>
@@ -157,16 +241,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,160 +566,630 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA9E9EE-20CB-488C-A45A-A967BB1A31C6}">
-  <dimension ref="C1:J8"/>
+  <dimension ref="C1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="3:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="3:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="3:10" ht="232" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="2" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="3:10" ht="188.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="2" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="3:12" ht="188.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="3:10" ht="174" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="3:12" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="3:10" ht="232" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="3:10" ht="232" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="3:10" ht="232" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="3:12" ht="246.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="3:10" ht="246.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="3:10" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="114">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
@@ -648,26 +1202,6 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
todos testes finalizados, separação dos tipos também
</commit_message>
<xml_diff>
--- a/Java/TestedeSistema.xlsx
+++ b/Java/TestedeSistema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csf14\Desktop\verival2Trab1\VeriVal2\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60489688-DCCE-47B8-8078-09787100A9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C73B22-184E-4F78-99C3-ED7D622BDA9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2DA30366-0FAA-42A7-BFD2-EF0DC84B3127}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="58">
   <si>
     <t>Descrição</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>O programa deve informar ao usuario que não é possivel excluir essa alocação, visto que está ocorrendo e impedi-la.</t>
+  </si>
+  <si>
+    <t>O usuario deve fazer uma reserva de sala, inserindo o numero 6, depois escolher o medico na posição 1 na lista, depois a sala de posição 7 na lista, e por fim, escolher a data inicial como 2020/11/14/11/00 e final como 2020/11/14/21/00</t>
+  </si>
+  <si>
+    <t>O programa permite que o usuario faça a reserva</t>
+  </si>
+  <si>
+    <t>Fracasso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ápos concertar o bug, o programa impede que um medico faça uma reserva numa data que colida com a data de uma reserva que esse mesmo medico fez numa sala diferente </t>
   </si>
 </sst>
 </file>
@@ -243,14 +255,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA9E9EE-20CB-488C-A45A-A967BB1A31C6}">
-  <dimension ref="C1:L28"/>
+  <dimension ref="C1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S42" sqref="S42"/>
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,18 +591,18 @@
         <v>0</v>
       </c>
       <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4"/>
+      <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
@@ -641,7 +653,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="1"/>
@@ -870,7 +882,7 @@
       </c>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
@@ -888,7 +900,7 @@
       </c>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
@@ -906,7 +918,7 @@
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
@@ -924,7 +936,7 @@
       </c>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="1" t="s">
         <v>48</v>
       </c>
@@ -942,7 +954,7 @@
       </c>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
         <v>40</v>
       </c>
@@ -960,7 +972,7 @@
       </c>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="1" t="s">
         <v>41</v>
       </c>
@@ -978,7 +990,7 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
@@ -996,7 +1008,7 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1014,7 +1026,7 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
@@ -1032,7 +1044,7 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1050,7 +1062,7 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="3:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
@@ -1068,7 +1080,7 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="3:10" ht="232" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C28" s="1" t="s">
         <v>52</v>
       </c>
@@ -1086,84 +1098,49 @@
       </c>
       <c r="J28" s="1"/>
     </row>
+    <row r="29" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L29" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="114">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
+  <mergeCells count="119">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
@@ -1188,20 +1165,82 @@
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
mudanças em alguns testes para ficar melhor, agora sim todos os testes estão finalizados
</commit_message>
<xml_diff>
--- a/Java/TestedeSistema.xlsx
+++ b/Java/TestedeSistema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csf14\Desktop\verival2Trab1\VeriVal2\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C73B22-184E-4F78-99C3-ED7D622BDA9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439BBD9D-E434-4DF3-A0BD-8A8FB560E913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2DA30366-0FAA-42A7-BFD2-EF0DC84B3127}"/>
   </bookViews>
@@ -256,10 +256,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -580,29 +580,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA9E9EE-20CB-488C-A45A-A967BB1A31C6}">
   <dimension ref="C1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="3:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="3"/>
       <c r="K1" s="1" t="s">
         <v>30</v>
       </c>
@@ -625,6 +625,8 @@
         <v>7</v>
       </c>
       <c r="J2" s="1"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="3:12" ht="188.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
@@ -643,6 +645,8 @@
         <v>7</v>
       </c>
       <c r="J3" s="1"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="3:12" ht="174" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
@@ -679,10 +683,12 @@
         <v>15</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="3"/>
+      <c r="I5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
@@ -701,6 +707,8 @@
         <v>7</v>
       </c>
       <c r="J6" s="1"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
@@ -719,6 +727,8 @@
         <v>7</v>
       </c>
       <c r="J7" s="1"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8" spans="3:12" ht="246.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
@@ -737,6 +747,8 @@
         <v>7</v>
       </c>
       <c r="J8" s="1"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
@@ -755,6 +767,8 @@
         <v>7</v>
       </c>
       <c r="J9" s="1"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
@@ -773,6 +787,8 @@
         <v>7</v>
       </c>
       <c r="J10" s="1"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
@@ -791,6 +807,8 @@
         <v>7</v>
       </c>
       <c r="J11" s="1"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
@@ -809,6 +827,8 @@
         <v>7</v>
       </c>
       <c r="J12" s="1"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
@@ -827,6 +847,8 @@
         <v>7</v>
       </c>
       <c r="J13" s="1"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
@@ -845,6 +867,8 @@
         <v>7</v>
       </c>
       <c r="J14" s="1"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
@@ -863,6 +887,8 @@
         <v>7</v>
       </c>
       <c r="J15" s="1"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
@@ -881,6 +907,8 @@
         <v>7</v>
       </c>
       <c r="J16" s="1"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
@@ -899,6 +927,8 @@
         <v>7</v>
       </c>
       <c r="J17" s="1"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
@@ -917,6 +947,8 @@
         <v>7</v>
       </c>
       <c r="J18" s="1"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
@@ -935,6 +967,8 @@
         <v>7</v>
       </c>
       <c r="J19" s="1"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
     <row r="20" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="1" t="s">
@@ -953,6 +987,8 @@
         <v>7</v>
       </c>
       <c r="J20" s="1"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
@@ -971,6 +1007,8 @@
         <v>7</v>
       </c>
       <c r="J21" s="1"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="1" t="s">
@@ -989,6 +1027,8 @@
         <v>7</v>
       </c>
       <c r="J22" s="1"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="1" t="s">
@@ -1007,6 +1047,8 @@
         <v>7</v>
       </c>
       <c r="J23" s="1"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
     </row>
     <row r="24" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C24" s="1" t="s">
@@ -1025,6 +1067,8 @@
         <v>7</v>
       </c>
       <c r="J24" s="1"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
     </row>
     <row r="25" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="1" t="s">
@@ -1043,6 +1087,8 @@
         <v>7</v>
       </c>
       <c r="J25" s="1"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
     </row>
     <row r="26" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="1" t="s">
@@ -1061,6 +1107,8 @@
         <v>7</v>
       </c>
       <c r="J26" s="1"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
     </row>
     <row r="27" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="1" t="s">
@@ -1079,6 +1127,8 @@
         <v>7</v>
       </c>
       <c r="J27" s="1"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="3:12" ht="232" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C28" s="1" t="s">
@@ -1097,6 +1147,8 @@
         <v>7</v>
       </c>
       <c r="J28" s="1"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
     </row>
     <row r="29" spans="3:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
@@ -1111,17 +1163,138 @@
         <v>55</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="3"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="1" t="s">
         <v>57</v>
       </c>
       <c r="L29" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="119">
+  <mergeCells count="145">
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="G29:H29"/>
@@ -1145,102 +1318,7 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>